<commit_message>
Added defineable schedule column widths
</commit_message>
<xml_diff>
--- a/excelFiles/Excel.xlsx
+++ b/excelFiles/Excel.xlsx
@@ -281,47 +281,47 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF8F001B"/>
+        <fgColor rgb="FF5A049B"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF403E7F"/>
+        <fgColor rgb="FF02193C"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF7B6C80"/>
+        <fgColor rgb="FF3A029B"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF0E3E4E"/>
+        <fgColor rgb="FF58481C"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF2D3588"/>
+        <fgColor rgb="FF319071"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF3B7C7A"/>
+        <fgColor rgb="FF7F1050"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF550259"/>
+        <fgColor rgb="FF801850"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF0B9C18"/>
+        <fgColor rgb="FF3A049C"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF58093D"/>
+        <fgColor rgb="FF99748C"/>
       </patternFill>
     </fill>
   </fills>
@@ -1531,6 +1531,17 @@
     <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="4" customWidth="1"/>
+    <col min="2" max="2" width="32" customWidth="1"/>
+    <col min="3" max="3" width="25" customWidth="1"/>
+    <col min="4" max="4" width="25" customWidth="1"/>
+    <col min="5" max="5" width="23" customWidth="1"/>
+    <col min="6" max="6" width="10.8" customWidth="1"/>
+    <col min="7" max="7" width="10.8" customWidth="1"/>
+    <col min="8" max="8" width="7" customWidth="1"/>
+    <col min="9" max="9" width="11" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="3" t="s">

</xml_diff>